<commit_message>
minor corrections in lifetime + changed LCI dataset for WET_BIOMASS
</commit_message>
<xml_diff>
--- a/dev/energyscope_data/CA-QC/unit_conversion_3.8.xlsx
+++ b/dev/energyscope_data/CA-QC/unit_conversion_3.8.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="770">
   <si>
     <t>Name</t>
   </si>
@@ -2282,7 +2282,7 @@
     <t>Refinery sludge LHV (2.453 MJ/kg): \cite{wernet2016}</t>
   </si>
   <si>
-    <t>LHV wet wood (8.279 MJ/kg): \cite{moret2017}</t>
+    <t>HHV manure (15 MJ/kg): \cite{marin-batista2020}, LHV-to-HHV ratio (0.95)</t>
   </si>
   <si>
     <t>LHV wood (15.4 MJ/kg): \cite{engineeringtoolbox2003}</t>
@@ -2316,9 +2316,6 @@
   </si>
   <si>
     <t>lignite HHV (3.89 kWh/kg): \cite{engineeringtoolbox2003}, LHV-to-HHV ratio (0.95)</t>
-  </si>
-  <si>
-    <t>HHV manure (15 MJ/kg): \cite{marin-batista2020}, LHV-to-HHV ratio (0.95)</t>
   </si>
   <si>
     <t>LHV natural gas (13.1 kWh/kg), density natural gas (0.777 kg/m3): \cite{engineeringtoolbox2003}</t>
@@ -21830,7 +21827,7 @@
         <v>603</v>
       </c>
       <c r="C940">
-        <f>1 * 3.6 / 8.279</f>
+        <f>1 * 3.6 / (0.95*15) / 1000000</f>
         <v>0</v>
       </c>
       <c r="D940" t="s">
@@ -22367,7 +22364,7 @@
         <v>608</v>
       </c>
       <c r="F967" t="s">
-        <v>767</v>
+        <v>755</v>
       </c>
     </row>
     <row r="968" spans="1:6">
@@ -22409,7 +22406,7 @@
         <v>608</v>
       </c>
       <c r="F969" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="970" spans="1:6">
@@ -22493,7 +22490,7 @@
         <v>608</v>
       </c>
       <c r="F973" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="974" spans="1:6">
@@ -22514,7 +22511,7 @@
         <v>607</v>
       </c>
       <c r="F974" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="975" spans="1:6">
@@ -22535,7 +22532,7 @@
         <v>610</v>
       </c>
       <c r="F975" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="976" spans="1:6">

</xml_diff>